<commit_message>
commit test excel changes
</commit_message>
<xml_diff>
--- a/excelFiles/lion-login-data.xlsx
+++ b/excelFiles/lion-login-data.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="135" windowWidth="14190" windowHeight="8010"/>
+    <workbookView xWindow="10545" yWindow="135" windowWidth="13725" windowHeight="8835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>password</t>
   </si>
@@ -24,9 +24,6 @@
     <t>venu</t>
   </si>
   <si>
-    <t>Error: The email address is badly formatted.</t>
-  </si>
-  <si>
     <t>venugopal.vellepu@walkingtree.tech</t>
   </si>
   <si>
@@ -61,6 +58,87 @@
   </si>
   <si>
     <t>submit</t>
+  </si>
+  <si>
+    <t>validateloginmessage</t>
+  </si>
+  <si>
+    <t>AcceptLoginAlert</t>
+  </si>
+  <si>
+    <t>venugopal@gmail.com</t>
+  </si>
+  <si>
+    <t>LoanPurpose</t>
+  </si>
+  <si>
+    <t>Refinance</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>OPT_contact Policy</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>SaveLoanPurpose</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>validateContactMessage</t>
+  </si>
+  <si>
+    <t>Contact Phone Number was left blank</t>
+  </si>
+  <si>
+    <t>acceptErrors</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>openAdressForm</t>
+  </si>
+  <si>
+    <t>Adress Line</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City </t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>closeAdressForm</t>
+  </si>
+  <si>
+    <t>adressForm</t>
+  </si>
+  <si>
+    <t>259 street, #342</t>
+  </si>
+  <si>
+    <t>Stephentown</t>
+  </si>
+  <si>
+    <t>Newyork</t>
+  </si>
+  <si>
+    <t>12168</t>
+  </si>
+  <si>
+    <t>PrimaryResidence</t>
+  </si>
+  <si>
+    <t>primary</t>
   </si>
 </sst>
 </file>
@@ -403,71 +481,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:18" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -492,43 +634,43 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>